<commit_message>
updated contributor-types, item-relation-types and resource-types
- added items to contributor-types, item-relation-types and resource-types
- updated hint_en column for all items in item-reladed-tipes
</commit_message>
<xml_diff>
--- a/nr_vocabularies/fixtures/contributor-types.xlsx
+++ b/nr_vocabularies/fixtures/contributor-types.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slasaj\Documents\GitHub\nr-vocabularies\nr_vocabularies\fixtures\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9402B05-6798-4AA7-A09D-5B0B60DEECEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="4065" yWindow="-13620" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="157">
   <si>
     <t>code</t>
   </si>
@@ -389,16 +398,106 @@
   </si>
   <si>
     <t>rsp</t>
+  </si>
+  <si>
+    <t>hosting-institution</t>
+  </si>
+  <si>
+    <t>hostující instituce</t>
+  </si>
+  <si>
+    <t>hosting institution</t>
+  </si>
+  <si>
+    <t>HostingInstitution</t>
+  </si>
+  <si>
+    <t>registration-agency</t>
+  </si>
+  <si>
+    <t>registrační agentura</t>
+  </si>
+  <si>
+    <t>registration agency</t>
+  </si>
+  <si>
+    <t>RegistrationAgency</t>
+  </si>
+  <si>
+    <t>registration-authority</t>
+  </si>
+  <si>
+    <t>registrační autorita</t>
+  </si>
+  <si>
+    <t>registration authority</t>
+  </si>
+  <si>
+    <t>RegistrationAuthority</t>
+  </si>
+  <si>
+    <t>related-person</t>
+  </si>
+  <si>
+    <t>související osoba</t>
+  </si>
+  <si>
+    <t>related person</t>
+  </si>
+  <si>
+    <t>RelatedPerson</t>
+  </si>
+  <si>
+    <t>sponsor</t>
+  </si>
+  <si>
+    <t>sponzor</t>
+  </si>
+  <si>
+    <t>spn</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
+  </si>
+  <si>
+    <t>work-package-leader</t>
+  </si>
+  <si>
+    <t>vedoucí pracovního balíku</t>
+  </si>
+  <si>
+    <t>work package leader</t>
+  </si>
+  <si>
+    <t>WorkPackageLeader</t>
+  </si>
+  <si>
+    <t>consultant</t>
+  </si>
+  <si>
+    <t>konzultant</t>
+  </si>
+  <si>
+    <t>csl</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>jiná</t>
+  </si>
+  <si>
+    <t>oth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -407,25 +506,10 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -530,82 +614,120 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Motiv Office">
       <a:dk1>
@@ -807,7 +929,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -826,7 +948,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -856,7 +978,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -882,7 +1004,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -908,7 +1030,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -934,7 +1056,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -960,7 +1082,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -986,7 +1108,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +1134,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1038,7 +1160,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1064,7 +1186,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1077,9 +1199,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1096,7 +1224,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1115,7 +1243,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1141,7 +1269,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1167,7 +1295,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1193,7 +1321,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1219,7 +1347,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1245,7 +1373,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1271,7 +1399,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1297,7 +1425,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1323,7 +1451,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1349,7 +1477,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1362,9 +1490,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1378,7 +1512,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1397,7 +1531,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1427,7 +1561,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1453,7 +1587,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1479,7 +1613,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1505,7 +1639,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1531,7 +1665,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1557,7 +1691,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1583,7 +1717,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1609,7 +1743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1635,7 +1769,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1648,44 +1782,53 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.65" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.8516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11.453125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3"/>
@@ -1695,14 +1838,14 @@
       <c r="H1" s="3"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" t="s" s="5">
+    <row r="2" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3"/>
@@ -1712,7 +1855,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" ht="13.65" customHeight="1">
+    <row r="3" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1723,7 +1866,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" ht="13.65" customHeight="1">
+    <row r="4" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1734,20 +1877,20 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" t="s" s="2">
+    <row r="5" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s" s="2">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="2"/>
@@ -1755,18 +1898,18 @@
       <c r="H5" s="4"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" t="s" s="6">
+    <row r="6" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s" s="8">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s" s="6">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" t="s" s="6">
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="6"/>
@@ -1774,18 +1917,18 @@
       <c r="H6" s="4"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" t="s" s="10">
+    <row r="7" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s" s="11">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s" s="10">
+      <c r="C7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" t="s" s="10">
+      <c r="E7" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="10"/>
@@ -1793,18 +1936,18 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" t="s" s="10">
+    <row r="8" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s" s="11">
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s" s="10">
+      <c r="C8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" t="s" s="10">
+      <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="10"/>
@@ -1812,20 +1955,20 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" t="s" s="10">
+    <row r="9" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s" s="11">
+      <c r="B9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s" s="10">
+      <c r="C9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s" s="10">
+      <c r="D9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s" s="10">
+      <c r="E9" s="10" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="10"/>
@@ -1833,20 +1976,20 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" t="s" s="10">
+    <row r="10" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s" s="11">
+      <c r="B10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s" s="10">
+      <c r="C10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s" s="10">
+      <c r="D10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s" s="10">
+      <c r="E10" s="10" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="10"/>
@@ -1854,20 +1997,20 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" ht="15.35" customHeight="1">
-      <c r="A11" t="s" s="10">
+    <row r="11" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s" s="11">
+      <c r="B11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s" s="10">
+      <c r="C11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s" s="10">
+      <c r="D11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s" s="10">
+      <c r="E11" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="10"/>
@@ -1875,20 +2018,20 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" ht="15.35" customHeight="1">
-      <c r="A12" t="s" s="10">
+    <row r="12" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s" s="11">
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s" s="10">
+      <c r="C12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s" s="10">
+      <c r="D12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s" s="10">
+      <c r="E12" s="10" t="s">
         <v>35</v>
       </c>
       <c r="F12" s="10"/>
@@ -1896,20 +2039,20 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" ht="15.35" customHeight="1">
-      <c r="A13" t="s" s="10">
+    <row r="13" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s" s="11">
+      <c r="B13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s" s="10">
+      <c r="C13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D13" t="s" s="10">
+      <c r="D13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E13" t="s" s="10">
+      <c r="E13" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="10"/>
@@ -1917,18 +2060,18 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" t="s" s="10">
+    <row r="14" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s" s="11">
+      <c r="B14" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C14" t="s" s="10">
+      <c r="C14" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" t="s" s="10">
+      <c r="E14" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="10"/>
@@ -1936,20 +2079,20 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" ht="15.35" customHeight="1">
-      <c r="A15" t="s" s="10">
+    <row r="15" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B15" t="s" s="11">
+      <c r="B15" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s" s="10">
+      <c r="C15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s" s="10">
+      <c r="D15" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E15" t="s" s="10">
+      <c r="E15" s="10" t="s">
         <v>49</v>
       </c>
       <c r="F15" s="10"/>
@@ -1957,20 +2100,20 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="10">
+    <row r="16" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s" s="11">
+      <c r="B16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C16" t="s" s="10">
+      <c r="C16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D16" t="s" s="10">
+      <c r="D16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E16" t="s" s="10">
+      <c r="E16" s="10" t="s">
         <v>53</v>
       </c>
       <c r="F16" s="10"/>
@@ -1978,18 +2121,18 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" t="s" s="10">
+    <row r="17" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B17" t="s" s="11">
+      <c r="B17" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C17" t="s" s="10">
+      <c r="C17" s="10" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" t="s" s="10">
+      <c r="E17" s="10" t="s">
         <v>57</v>
       </c>
       <c r="F17" s="10"/>
@@ -1997,20 +2140,20 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" ht="15.35" customHeight="1">
-      <c r="A18" t="s" s="10">
+    <row r="18" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B18" t="s" s="11">
+      <c r="B18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C18" t="s" s="10">
+      <c r="C18" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D18" t="s" s="10">
+      <c r="D18" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E18" t="s" s="10">
+      <c r="E18" s="10" t="s">
         <v>62</v>
       </c>
       <c r="F18" s="10"/>
@@ -2018,18 +2161,18 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="10">
+    <row r="19" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B19" t="s" s="11">
+      <c r="B19" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C19" t="s" s="10">
+      <c r="C19" s="10" t="s">
         <v>63</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" t="s" s="10">
+      <c r="E19" s="10" t="s">
         <v>65</v>
       </c>
       <c r="F19" s="10"/>
@@ -2037,17 +2180,17 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" t="s" s="10">
+    <row r="20" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B20" t="s" s="11">
+      <c r="B20" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C20" t="s" s="10">
+      <c r="C20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D20" t="s" s="10">
+      <c r="D20" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E20" s="4"/>
@@ -2056,17 +2199,17 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" ht="15.35" customHeight="1">
-      <c r="A21" t="s" s="10">
+    <row r="21" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B21" t="s" s="11">
+      <c r="B21" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C21" t="s" s="10">
+      <c r="C21" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D21" t="s" s="10">
+      <c r="D21" s="10" t="s">
         <v>71</v>
       </c>
       <c r="E21" s="4"/>
@@ -2075,17 +2218,17 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" ht="15.35" customHeight="1">
-      <c r="A22" t="s" s="10">
+    <row r="22" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B22" t="s" s="11">
+      <c r="B22" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C22" t="s" s="10">
+      <c r="C22" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D22" t="s" s="10">
+      <c r="D22" s="10" t="s">
         <v>74</v>
       </c>
       <c r="E22" s="4"/>
@@ -2094,14 +2237,14 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" ht="15.35" customHeight="1">
-      <c r="A23" t="s" s="10">
+    <row r="23" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B23" t="s" s="11">
+      <c r="B23" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C23" t="s" s="10">
+      <c r="C23" s="10" t="s">
         <v>77</v>
       </c>
       <c r="D23" s="4"/>
@@ -2111,17 +2254,17 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" ht="15.35" customHeight="1">
-      <c r="A24" t="s" s="10">
+    <row r="24" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B24" t="s" s="11">
+      <c r="B24" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C24" t="s" s="10">
+      <c r="C24" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D24" t="s" s="10">
+      <c r="D24" s="10" t="s">
         <v>80</v>
       </c>
       <c r="E24" s="4"/>
@@ -2130,17 +2273,17 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" ht="15.35" customHeight="1">
-      <c r="A25" t="s" s="10">
+    <row r="25" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B25" t="s" s="11">
+      <c r="B25" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C25" t="s" s="10">
+      <c r="C25" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D25" t="s" s="10">
+      <c r="D25" s="10" t="s">
         <v>83</v>
       </c>
       <c r="E25" s="4"/>
@@ -2149,17 +2292,17 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" ht="15.35" customHeight="1">
-      <c r="A26" t="s" s="10">
+    <row r="26" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B26" t="s" s="11">
+      <c r="B26" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C26" t="s" s="10">
+      <c r="C26" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D26" t="s" s="10">
+      <c r="D26" s="10" t="s">
         <v>86</v>
       </c>
       <c r="E26" s="4"/>
@@ -2168,17 +2311,17 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" ht="15.35" customHeight="1">
-      <c r="A27" t="s" s="10">
+    <row r="27" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B27" t="s" s="11">
+      <c r="B27" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C27" t="s" s="10">
+      <c r="C27" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D27" t="s" s="10">
+      <c r="D27" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E27" s="4"/>
@@ -2187,17 +2330,17 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" t="s" s="10">
+    <row r="28" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B28" t="s" s="11">
+      <c r="B28" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C28" t="s" s="10">
+      <c r="C28" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D28" t="s" s="10">
+      <c r="D28" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E28" s="4"/>
@@ -2206,17 +2349,17 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" ht="15.35" customHeight="1">
-      <c r="A29" t="s" s="10">
+    <row r="29" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B29" t="s" s="11">
+      <c r="B29" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C29" t="s" s="10">
+      <c r="C29" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D29" t="s" s="10">
+      <c r="D29" s="10" t="s">
         <v>95</v>
       </c>
       <c r="E29" s="4"/>
@@ -2225,17 +2368,17 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" ht="15.35" customHeight="1">
-      <c r="A30" t="s" s="10">
+    <row r="30" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B30" t="s" s="11">
+      <c r="B30" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C30" t="s" s="10">
+      <c r="C30" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D30" t="s" s="10">
+      <c r="D30" s="10" t="s">
         <v>98</v>
       </c>
       <c r="E30" s="4"/>
@@ -2244,17 +2387,17 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" ht="15.35" customHeight="1">
-      <c r="A31" t="s" s="10">
+    <row r="31" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B31" t="s" s="11">
+      <c r="B31" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C31" t="s" s="10">
+      <c r="C31" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D31" t="s" s="10">
+      <c r="D31" s="10" t="s">
         <v>101</v>
       </c>
       <c r="E31" s="4"/>
@@ -2263,17 +2406,17 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" t="s" s="10">
+    <row r="32" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B32" t="s" s="11">
+      <c r="B32" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C32" t="s" s="10">
+      <c r="C32" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D32" t="s" s="10">
+      <c r="D32" s="10" t="s">
         <v>104</v>
       </c>
       <c r="E32" s="4"/>
@@ -2282,17 +2425,17 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" ht="15.35" customHeight="1">
-      <c r="A33" t="s" s="10">
+    <row r="33" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B33" t="s" s="11">
+      <c r="B33" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C33" t="s" s="10">
+      <c r="C33" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D33" t="s" s="10">
+      <c r="D33" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E33" s="4"/>
@@ -2301,17 +2444,17 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" ht="15.35" customHeight="1">
-      <c r="A34" t="s" s="10">
+    <row r="34" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B34" t="s" s="10">
+      <c r="B34" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C34" t="s" s="10">
+      <c r="C34" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D34" t="s" s="10">
+      <c r="D34" s="10" t="s">
         <v>110</v>
       </c>
       <c r="E34" s="4"/>
@@ -2320,17 +2463,17 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" ht="15.35" customHeight="1">
-      <c r="A35" t="s" s="10">
+    <row r="35" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B35" t="s" s="10">
+      <c r="B35" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C35" t="s" s="10">
+      <c r="C35" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D35" t="s" s="10">
+      <c r="D35" s="10" t="s">
         <v>113</v>
       </c>
       <c r="E35" s="4"/>
@@ -2339,17 +2482,17 @@
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" ht="15.35" customHeight="1">
-      <c r="A36" t="s" s="10">
+    <row r="36" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B36" t="s" s="10">
+      <c r="B36" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C36" t="s" s="10">
+      <c r="C36" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D36" t="s" s="10">
+      <c r="D36" s="10" t="s">
         <v>116</v>
       </c>
       <c r="E36" s="4"/>
@@ -2358,17 +2501,17 @@
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" ht="15.35" customHeight="1">
-      <c r="A37" t="s" s="10">
+    <row r="37" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B37" t="s" s="10">
+      <c r="B37" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C37" t="s" s="10">
+      <c r="C37" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D37" t="s" s="10">
+      <c r="D37" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E37" s="4"/>
@@ -2377,17 +2520,17 @@
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" ht="15.35" customHeight="1">
-      <c r="A38" t="s" s="10">
+    <row r="38" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B38" t="s" s="10">
+      <c r="B38" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C38" t="s" s="10">
+      <c r="C38" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D38" t="s" s="10">
+      <c r="D38" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E38" s="4"/>
@@ -2396,17 +2539,17 @@
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" ht="15.35" customHeight="1">
-      <c r="A39" t="s" s="12">
+    <row r="39" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B39" t="s" s="12">
+      <c r="B39" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C39" t="s" s="12">
+      <c r="C39" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="D39" t="s" s="12">
+      <c r="D39" s="12" t="s">
         <v>125</v>
       </c>
       <c r="E39" s="4"/>
@@ -2415,95 +2558,167 @@
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" ht="13.65" customHeight="1">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="4"/>
+    <row r="40" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="14"/>
+      <c r="E40" s="15" t="s">
+        <v>129</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" ht="13.65" customHeight="1">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
+    <row r="41" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15" t="s">
+        <v>133</v>
+      </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" ht="13.65" customHeight="1">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
+    <row r="42" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15" t="s">
+        <v>137</v>
+      </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" ht="13.65" customHeight="1">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+    <row r="43" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15" t="s">
+        <v>141</v>
+      </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" ht="13.65" customHeight="1">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
+    <row r="44" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>145</v>
+      </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" ht="13.65" customHeight="1">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+    <row r="45" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>149</v>
+      </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" ht="13.65" customHeight="1">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
+    <row r="46" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>153</v>
+      </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" ht="13.65" customHeight="1">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
+    <row r="47" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>153</v>
+      </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" ht="13.65" customHeight="1">
+    <row r="48" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2514,7 +2729,7 @@
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" ht="13.65" customHeight="1">
+    <row r="49" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2525,18 +2740,18 @@
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
-    <row r="50" ht="15.35" customHeight="1">
+    <row r="50" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="14"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
     </row>
-    <row r="51" ht="13.65" customHeight="1">
+    <row r="51" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2547,7 +2762,7 @@
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" ht="13.65" customHeight="1">
+    <row r="52" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2558,7 +2773,7 @@
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
     </row>
-    <row r="53" ht="13.65" customHeight="1">
+    <row r="53" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2569,7 +2784,7 @@
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
     </row>
-    <row r="54" ht="13.65" customHeight="1">
+    <row r="54" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2580,18 +2795,18 @@
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
     </row>
-    <row r="55" ht="15.35" customHeight="1">
+    <row r="55" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="14"/>
+      <c r="E55" s="13"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
     </row>
-    <row r="56" ht="13.65" customHeight="1">
+    <row r="56" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2602,7 +2817,7 @@
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
     </row>
-    <row r="57" ht="13.65" customHeight="1">
+    <row r="57" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2613,7 +2828,7 @@
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
     </row>
-    <row r="58" ht="13.65" customHeight="1">
+    <row r="58" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2624,7 +2839,7 @@
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
     </row>
-    <row r="59" ht="13.65" customHeight="1">
+    <row r="59" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2635,7 +2850,7 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" ht="13.65" customHeight="1">
+    <row r="60" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2646,7 +2861,7 @@
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" ht="13.65" customHeight="1">
+    <row r="61" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -2657,18 +2872,18 @@
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
     </row>
-    <row r="62" ht="15.35" customHeight="1">
+    <row r="62" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
     </row>
-    <row r="63" ht="13.65" customHeight="1">
+    <row r="63" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -2679,7 +2894,7 @@
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
     </row>
-    <row r="64" ht="13.65" customHeight="1">
+    <row r="64" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2690,7 +2905,7 @@
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" ht="13.65" customHeight="1">
+    <row r="65" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -2701,7 +2916,7 @@
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
     </row>
-    <row r="66" ht="13.65" customHeight="1">
+    <row r="66" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -2712,7 +2927,7 @@
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
     </row>
-    <row r="67" ht="13.65" customHeight="1">
+    <row r="67" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -2723,7 +2938,7 @@
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" ht="13.65" customHeight="1">
+    <row r="68" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -2734,7 +2949,7 @@
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
-    <row r="69" ht="13.65" customHeight="1">
+    <row r="69" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -2745,7 +2960,7 @@
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
     </row>
-    <row r="70" ht="13.65" customHeight="1">
+    <row r="70" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -2756,7 +2971,7 @@
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
-    <row r="71" ht="13.65" customHeight="1">
+    <row r="71" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2767,7 +2982,7 @@
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
-    <row r="72" ht="13.65" customHeight="1">
+    <row r="72" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -2778,7 +2993,7 @@
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" ht="13.65" customHeight="1">
+    <row r="73" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -2789,18 +3004,18 @@
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" ht="15.35" customHeight="1">
+    <row r="74" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" ht="13.65" customHeight="1">
+    <row r="75" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -2811,7 +3026,7 @@
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" ht="13.65" customHeight="1">
+    <row r="76" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -2822,7 +3037,7 @@
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" ht="13.65" customHeight="1">
+    <row r="77" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -2833,7 +3048,7 @@
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
     </row>
-    <row r="78" ht="13.65" customHeight="1">
+    <row r="78" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -2844,7 +3059,7 @@
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
     </row>
-    <row r="79" ht="13.65" customHeight="1">
+    <row r="79" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -2855,7 +3070,7 @@
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
     </row>
-    <row r="80" ht="13.65" customHeight="1">
+    <row r="80" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -2866,7 +3081,7 @@
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
     </row>
-    <row r="81" ht="13.65" customHeight="1">
+    <row r="81" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -2877,7 +3092,7 @@
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
     </row>
-    <row r="82" ht="13.65" customHeight="1">
+    <row r="82" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -2888,7 +3103,7 @@
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
     </row>
-    <row r="83" ht="13.65" customHeight="1">
+    <row r="83" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -2899,7 +3114,7 @@
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
     </row>
-    <row r="84" ht="13.65" customHeight="1">
+    <row r="84" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -2910,7 +3125,7 @@
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
     </row>
-    <row r="85" ht="13.65" customHeight="1">
+    <row r="85" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -2921,7 +3136,7 @@
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
     </row>
-    <row r="86" ht="13.65" customHeight="1">
+    <row r="86" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -2932,7 +3147,7 @@
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
     </row>
-    <row r="87" ht="13.65" customHeight="1">
+    <row r="87" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -2943,7 +3158,7 @@
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
     </row>
-    <row r="88" ht="13.65" customHeight="1">
+    <row r="88" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -2954,7 +3169,7 @@
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" ht="13.65" customHeight="1">
+    <row r="89" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -2965,7 +3180,7 @@
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
     </row>
-    <row r="90" ht="13.65" customHeight="1">
+    <row r="90" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -2976,7 +3191,7 @@
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" ht="13.65" customHeight="1">
+    <row r="91" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -2987,7 +3202,7 @@
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" ht="13.65" customHeight="1">
+    <row r="92" spans="1:9" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -2998,20 +3213,20 @@
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" ht="15.35" customHeight="1">
+    <row r="93" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
-      <c r="D93" s="14"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="14"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05278" bottom="1.05278" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Sheet1</oddHeader>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>